<commit_message>
add yuli new cognates experiment - streched (v4) vs not (v3)
</commit_message>
<xml_diff>
--- a/statistical_clf_process/clf_results.xlsx
+++ b/statistical_clf_process/clf_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsofteur-my.sharepoint.com/personal/t-deangeckt_microsoft_com/Documents/Personal/HU/nlp_lab/code_and_data/miami_bangor_cs_cls/statistical_clf_process/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="11_F25DC773A252ABDACC10487611DB4C985ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C62383A4-8FA6-44F2-B702-E6A8DE6548A2}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="11_F25DC773A252ABDACC10487611DB4C985ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEE2F0E7-87F0-4E96-AA6E-ED8D202D4B28}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>pos tag + len + cognate</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>pos tag + len + cognatehood (v2) + words (100)</t>
+  </si>
+  <si>
+    <t>pos tag + len + cognatehood (v3)</t>
+  </si>
+  <si>
+    <t>pos tag + len + cognatehood (v3) + words (100)</t>
+  </si>
+  <si>
+    <t>pos tag + len + cognatehood (v4)</t>
+  </si>
+  <si>
+    <t>pos tag + len + cognatehood (v4) + words (100)</t>
   </si>
 </sst>
 </file>
@@ -802,7 +814,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$12</c:f>
+              <c:f>Sheet1!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -881,7 +893,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$13:$A$20</c:f>
+              <c:f>Sheet1!$A$17:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -913,7 +925,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$B$20</c:f>
+              <c:f>Sheet1!$B$17:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -955,7 +967,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$12</c:f>
+              <c:f>Sheet1!$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1034,7 +1046,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$13:$A$20</c:f>
+              <c:f>Sheet1!$A$17:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1066,7 +1078,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$13:$C$20</c:f>
+              <c:f>Sheet1!$C$17:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2405,7 +2417,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2435,13 +2447,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>453390</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2733,10 +2745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C28" sqref="A1:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2822,7 +2834,7 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0.86399999999999999</v>
       </c>
       <c r="C7">
@@ -2854,110 +2866,206 @@
         <v>8.7591240875912479</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>0.86</v>
+      </c>
+      <c r="C10">
+        <f>((1-B2)-(1-B10)) / (1-B2) * 100</f>
+        <v>6.0402684563758431</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="C11">
+        <f>((1-B2)-(1-B11)) / (1-B2) * 100</f>
+        <v>8.7248322147651081</v>
+      </c>
+    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2</v>
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="C12">
+        <f>((1-B2)-(1-B12)) / (1-B2) * 100</f>
+        <v>5.3691275167785273</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>0.5</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="C13">
-        <f>((1-B13)-(1-B13)) / (1-B13) * 100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="C14">
-        <f>((1-B13)-(1-B14)) / (1-B13) * 100</f>
-        <v>43.399999999999991</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="C15">
-        <f>((1-B13)-(1-B15)) / (1-B13) * 100</f>
-        <v>46.8</v>
+        <f>((1-B2)-(1-B13)) / (1-B2) * 100</f>
+        <v>8.0536912751677914</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="C16">
-        <f>((1-B13)-(1-B16)) / (1-B13) * 100</f>
-        <v>46.599999999999994</v>
+      <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>0.752</v>
+        <v>0.5</v>
       </c>
       <c r="C17">
-        <f>((1-B13)-(1-B17)) / (1-B13) * 100</f>
-        <v>50.4</v>
+        <f>((1-B17)-(1-B17)) / (1-B17) * 100</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B18">
-        <v>0.753</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="C18">
-        <f>((1-B13)-(1-B18)) / (1-B13) * 100</f>
-        <v>50.6</v>
+        <f>((1-B17)-(1-B18)) / (1-B17) * 100</f>
+        <v>43.399999999999991</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>0.73399999999999999</v>
       </c>
       <c r="C19">
-        <f>((1-B13)-(1-B19)) / (1-B13) * 100</f>
+        <f>((1-B17)-(1-B19)) / (1-B17) * 100</f>
         <v>46.8</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="C20">
+        <f>((1-B17)-(1-B20)) / (1-B17) * 100</f>
+        <v>46.599999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>0.752</v>
+      </c>
+      <c r="C21">
+        <f>((1-B17)-(1-B21)) / (1-B17) * 100</f>
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.753</v>
+      </c>
+      <c r="C22">
+        <f>((1-B17)-(1-B22)) / (1-B17) * 100</f>
+        <v>50.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="C23">
+        <f>((1-B17)-(1-B23)) / (1-B17) * 100</f>
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>11</v>
       </c>
-      <c r="B20">
+      <c r="B24">
         <v>0.745</v>
       </c>
-      <c r="C20">
-        <f>((1-B13)-(1-B20)) / (1-B13) * 100</f>
+      <c r="C24">
+        <f>((1-B17)-(1-B24)) / (1-B17) * 100</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="C25">
+        <f>((1-B17)-(1-B25)) / (1-B17) * 100</f>
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>0.747</v>
+      </c>
+      <c r="C26">
+        <f>((1-B17)-(1-B26)) / (1-B17) * 100</f>
+        <v>49.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="C27">
+        <f>((1-B17)-(1-B27)) / (1-B17) * 100</f>
+        <v>47.599999999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>0.745</v>
+      </c>
+      <c r="C28">
+        <f>((1-B17)-(1-B28)) / (1-B17) * 100</f>
         <v>49</v>
       </c>
     </row>

</xml_diff>